<commit_message>
all new changes applied
</commit_message>
<xml_diff>
--- a/wwwroot/data/kafe.xlsx
+++ b/wwwroot/data/kafe.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28803"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28814"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6BAD49A9-747B-4159-848C-29D5FA443AF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{27C9BD3E-47B5-49E9-97B9-7D7FDC365C4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,10 +36,10 @@
     <t>اسپرسو ربوستا 100</t>
   </si>
   <si>
-    <t>تک :‌   43T</t>
-  </si>
-  <si>
-    <t>دبل :‌   59T</t>
+    <t>قیمت تک :‌   43T</t>
+  </si>
+  <si>
+    <t>قیمت دبل :‌   59T</t>
   </si>
   <si>
     <t>coffe</t>
@@ -48,70 +48,70 @@
     <t>اسپرسو ترکیبی 30-70</t>
   </si>
   <si>
-    <t>تک :‌   48T</t>
-  </si>
-  <si>
-    <t>دبل :‌   64T</t>
+    <t>قیمت تک :‌   48T</t>
+  </si>
+  <si>
+    <t>قیمت دبل :‌   64T</t>
   </si>
   <si>
     <t>اسپرسو عربیکا 100</t>
   </si>
   <si>
-    <t>تک :‌   58T</t>
-  </si>
-  <si>
-    <t>دبل :‌   78T</t>
+    <t>قیمت تک :‌   58T</t>
+  </si>
+  <si>
+    <t>قیمت دبل :‌   78T</t>
   </si>
   <si>
     <t>اسپرسو رومانو</t>
   </si>
   <si>
-    <t>75T</t>
+    <t>قیمت :   75T</t>
   </si>
   <si>
     <t>آیس کافی</t>
   </si>
   <si>
-    <t>65T</t>
+    <t>قیمت :   65T</t>
   </si>
   <si>
     <t>امریکانو</t>
   </si>
   <si>
-    <t>گرم :   65T</t>
-  </si>
-  <si>
-    <t>سرد :   65T</t>
+    <t>قیمت گرم :   65T</t>
+  </si>
+  <si>
+    <t>قیمت سرد :   65T</t>
   </si>
   <si>
     <t>کورتادو</t>
   </si>
   <si>
-    <t>گرم :   74T</t>
+    <t>قیمت گرم :   74T</t>
   </si>
   <si>
     <t>کاپوچینو</t>
   </si>
   <si>
-    <t>گرم :   79T</t>
+    <t>قیمت گرم :   79T</t>
   </si>
   <si>
     <t>لاته</t>
   </si>
   <si>
-    <t>گرم :   89T</t>
-  </si>
-  <si>
-    <t>سرد :   89T</t>
+    <t>قیمت گرم :   89T</t>
+  </si>
+  <si>
+    <t>قیمت سرد :   89T</t>
   </si>
   <si>
     <t>ماکیاتو</t>
   </si>
   <si>
-    <t>گرم :   108T</t>
-  </si>
-  <si>
-    <t>سرد :   108T</t>
+    <t>قیمت گرم :   108T</t>
+  </si>
+  <si>
+    <t>قیمت سرد :   108T</t>
   </si>
   <si>
     <t>کارامل، فندق،‌ وانیل،‌ نارگیل، شکلات، نوتلا</t>
@@ -120,7 +120,7 @@
     <t>هانی ماکیاتو</t>
   </si>
   <si>
-    <t>گرم :   115T</t>
+    <t>قیمت گرم :   115T</t>
   </si>
   <si>
     <t>موکا</t>
@@ -129,19 +129,19 @@
     <t>آفوگاتو</t>
   </si>
   <si>
-    <t>105T</t>
+    <t>قیمت :   105T</t>
   </si>
   <si>
     <t>نسکافه</t>
   </si>
   <si>
-    <t>85T</t>
+    <t>قیمت :   85T</t>
   </si>
   <si>
     <t>فرانسه</t>
   </si>
   <si>
-    <t>69T</t>
+    <t>قیمت :   69T</t>
   </si>
   <si>
     <t>یونانی</t>
@@ -153,7 +153,7 @@
     <t>هات چاکلت</t>
   </si>
   <si>
-    <t>98T</t>
+    <t>قیمت :   98T</t>
   </si>
   <si>
     <t>hot drink</t>
@@ -168,7 +168,7 @@
     <t>نوتلا چاکلت</t>
   </si>
   <si>
-    <t>115T</t>
+    <t>قیمت :   115T</t>
   </si>
   <si>
     <t>ماسالا</t>
@@ -180,13 +180,13 @@
     <t>شیر کاکائو</t>
   </si>
   <si>
-    <t>79T</t>
+    <t>قیمت :   79T</t>
   </si>
   <si>
     <t>شیر عسل</t>
   </si>
   <si>
-    <t>89T</t>
+    <t>قیمت :   89T</t>
   </si>
   <si>
     <t>سلامت</t>
@@ -213,19 +213,19 @@
     <t>چای کلاسیک</t>
   </si>
   <si>
-    <t>45T</t>
+    <t>قیمت :   45T</t>
   </si>
   <si>
     <t>چای سبز</t>
   </si>
   <si>
-    <t>55T</t>
+    <t>قیمت :   55T</t>
   </si>
   <si>
     <t>چای ترش</t>
   </si>
   <si>
-    <t>58T</t>
+    <t>قیمت :   58T</t>
   </si>
   <si>
     <t>چای زعفران</t>
@@ -234,7 +234,7 @@
     <t>سیب کلاسیک</t>
   </si>
   <si>
-    <t>110T</t>
+    <t>قیمت :   110T</t>
   </si>
   <si>
     <t>snack</t>
@@ -243,25 +243,25 @@
     <t>سیب سوخاری</t>
   </si>
   <si>
-    <t>189T</t>
+    <t>قیمت :   189T</t>
   </si>
   <si>
     <t>فیله استریپس</t>
   </si>
   <si>
-    <t>269T</t>
+    <t>قیمت :   269T</t>
   </si>
   <si>
     <t>کیک روز</t>
   </si>
   <si>
-    <t>68T</t>
+    <t>قیمت :   68T</t>
   </si>
   <si>
     <t>کوکی</t>
   </si>
   <si>
-    <t>4T</t>
+    <t>قیمت :   --</t>
   </si>
   <si>
     <t>میلک شیک</t>
@@ -273,25 +273,25 @@
     <t>موز شکلات</t>
   </si>
   <si>
-    <t>165T</t>
+    <t>قیمت :   165T</t>
   </si>
   <si>
     <t>نوتلا</t>
   </si>
   <si>
-    <t>170T</t>
+    <t>قیمت :   170T</t>
   </si>
   <si>
     <t>وانیل</t>
   </si>
   <si>
-    <t>138T</t>
+    <t>قیمت :   138T</t>
   </si>
   <si>
     <t>توت فرنگی</t>
   </si>
   <si>
-    <t>148T</t>
+    <t>قیمت :   148T</t>
   </si>
   <si>
     <t>بادام زمینی</t>
@@ -303,7 +303,7 @@
     <t>معجون پروتئین</t>
   </si>
   <si>
-    <t>275T</t>
+    <t>قیمت :   275T</t>
   </si>
   <si>
     <t>پروتئین وی ساشه، گردو، کره بادام زمینی، خرما، عسل، موز</t>
@@ -318,7 +318,7 @@
     <t>موهیتو</t>
   </si>
   <si>
-    <t>95T</t>
+    <t>قیمت :   95T</t>
   </si>
   <si>
     <t>رِد من</t>
@@ -327,7 +327,7 @@
     <t>اسپایسی دی</t>
   </si>
   <si>
-    <t>118T</t>
+    <t>قیمت :   118T</t>
   </si>
   <si>
     <t>خیار سکنجبین</t>
@@ -342,13 +342,13 @@
     <t>نوستالژی</t>
   </si>
   <si>
-    <t>120T</t>
+    <t>قیمت :   120T</t>
   </si>
   <si>
     <t>سیب آبی</t>
   </si>
   <si>
-    <t>145T</t>
+    <t>قیمت :   145T</t>
   </si>
   <si>
     <t>smothie</t>
@@ -357,7 +357,7 @@
     <t>چشمک</t>
   </si>
   <si>
-    <t>195T</t>
+    <t>قیمت :   195T</t>
   </si>
 </sst>
 </file>
@@ -732,7 +732,7 @@
   <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1"/>

</xml_diff>